<commit_message>
impl- markdown in the intro
</commit_message>
<xml_diff>
--- a/plot/global_dataframe.xlsx
+++ b/plot/global_dataframe.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -426,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX3"/>
+  <dimension ref="A1:AX4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,20 +662,14 @@
           <t>KB07 FC 1 1 Dez2019</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Dez2019</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>6145885.6</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1394515.6</t>
-        </is>
+      <c r="C2" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6145885.6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1394515.6</v>
       </c>
       <c r="F2" t="n">
         <v>1.629787234042553</v>
@@ -818,20 +816,14 @@
           <t>KB08 FC 2 1 Mar2020</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Mar20</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>6145844.9</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1394446</t>
-        </is>
+      <c r="C3" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6145844.9</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1394446</v>
       </c>
       <c r="F3" t="n">
         <v>1.223595505617977</v>
@@ -968,6 +960,68 @@
       <c r="AX3" t="n">
         <v>0</v>
       </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="n">
+        <v>0.621</v>
+      </c>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Interactive Plotter cum_gsd plot
</commit_message>
<xml_diff>
--- a/plot/global_dataframe.xlsx
+++ b/plot/global_dataframe.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -53,23 +53,22 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -962,6 +961,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>